<commit_message>
Improved documentation in Test Suite
</commit_message>
<xml_diff>
--- a/excel/TestSuiteKey.xlsx
+++ b/excel/TestSuiteKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A42443-BDF1-4CE7-BA6D-6FE27E242BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99E6EFC-7787-4080-92D2-1BB3AF3EF061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="883" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="25950" yWindow="7155" windowWidth="8850" windowHeight="4830" tabRatio="883" firstSheet="13" activeTab="14" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -102,27 +102,16 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> type: check
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">alt_cells:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="18"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> - F10
+          <t xml:space="preserve"> type: check</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
       </text>
@@ -1150,7 +1139,7 @@
  score: 1.5
  type: formula
  prereq:
-  - B9
+  - B8
 </t>
         </r>
       </text>
@@ -3222,7 +3211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="80">
   <si>
     <t>Number</t>
   </si>
@@ -3459,6 +3448,10 @@
   </si>
   <si>
     <t>At least try something.</t>
+  </si>
+  <si>
+    <t>NOTE: Values in columns B and C are here for understanding only.
+Actual evaluation of formula given in column A happens on the submission cols B&amp;C</t>
   </si>
 </sst>
 </file>
@@ -3549,9 +3542,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3869,8 +3865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{713B2A36-CAF8-2349-917C-6D8074132DA3}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4102,7 +4098,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4114,7 +4110,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>B2+C2</f>
+        <f t="shared" ref="A2:A9" si="0">B2+C2</f>
         <v>300</v>
       </c>
       <c r="B2">
@@ -4129,7 +4125,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>B3+C3</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B3">
@@ -4144,7 +4140,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>B4+C4</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B4">
@@ -4159,7 +4155,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>B5+C5</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B5">
@@ -4174,7 +4170,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>B6+C6</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B6">
@@ -4189,7 +4185,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>B7+C7</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B7">
@@ -4204,7 +4200,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>B8+C8</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B8">
@@ -4219,7 +4215,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f>B9+C9</f>
+        <f t="shared" si="0"/>
         <v>300</v>
       </c>
       <c r="B9">
@@ -4355,7 +4351,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4547,8 +4543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2DD034-B648-46D5-BADB-A1FE81998501}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4958,7 +4954,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5166,7 +5162,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5414,7 +5410,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5657,10 +5653,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F753B85-5CB9-481B-8C77-51ACF6917C73}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5812,6 +5808,11 @@
         <v>8888</v>
       </c>
     </row>
+    <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="D15" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
#12 columns in checkorder tabs order independent
</commit_message>
<xml_diff>
--- a/excel/TestSuiteKey.xlsx
+++ b/excel/TestSuiteKey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Notes\AutoGraderProject\pysheetgrader-core\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16E25C7-A197-43D1-9AEB-614810D8F893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287B546F-DF95-4D85-BC7F-90A57694B65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7008" yWindow="7032" windowWidth="8856" windowHeight="4836" tabRatio="883" firstSheet="4" activeTab="5" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
+    <workbookView xWindow="37995" yWindow="9225" windowWidth="8850" windowHeight="4830" tabRatio="883" firstSheet="13" activeTab="16" xr2:uid="{6E72627C-1CB6-4848-9B50-C1295434D515}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="1" r:id="rId1"/>
@@ -3400,12 +3400,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="83">
   <si>
     <t>Number</t>
-  </si>
-  <si>
-    <t>Sheetname</t>
   </si>
   <si>
     <t>Constant Samples</t>
@@ -3647,6 +3644,12 @@
   </si>
   <si>
     <t>A12</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>min-work</t>
   </si>
 </sst>
 </file>
@@ -4061,7 +4064,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4074,13 +4077,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
-      </c>
-      <c r="D1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -4088,13 +4091,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -4102,13 +4105,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -4116,13 +4119,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -4130,13 +4133,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -4144,13 +4147,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -4158,13 +4161,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -4172,13 +4175,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -4186,13 +4189,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -4215,7 +4218,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -4223,10 +4226,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -4234,7 +4237,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -4242,7 +4245,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -4250,7 +4253,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -4258,7 +4261,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -4266,7 +4269,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -4274,7 +4277,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -4282,7 +4285,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -4290,7 +4293,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -4298,7 +4301,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -4306,7 +4309,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -4314,7 +4317,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -4339,29 +4342,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <f>B2 / 10</f>
@@ -4370,7 +4373,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <f xml:space="preserve">  ROUNDUP(B2 / 100, 0)</f>
@@ -4379,7 +4382,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -4387,7 +4390,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <f xml:space="preserve"> B6 / 1000</f>
@@ -4396,7 +4399,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <f>B6 * 3.28084</f>
@@ -4405,14 +4408,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -4423,7 +4426,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B11">
         <f>B2 / 1000</f>
@@ -4432,7 +4435,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12">
         <f>SUM(B2:B4)</f>
@@ -4441,7 +4444,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <f>SUM(B2:B4) + 2</f>
@@ -4450,7 +4453,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <f>B2 / 5</f>
@@ -4459,7 +4462,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <f>B2 / 10</f>
@@ -4488,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4496,7 +4499,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4504,7 +4507,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4512,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4520,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4528,7 +4531,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4536,7 +4539,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4544,7 +4547,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4552,7 +4555,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4573,7 +4576,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -4588,7 +4591,7 @@
         <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -4603,7 +4606,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4618,7 +4621,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4633,7 +4636,7 @@
         <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4648,7 +4651,7 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4663,7 +4666,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4678,7 +4681,7 @@
         <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -4693,7 +4696,7 @@
         <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -4722,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4730,7 +4733,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4738,7 +4741,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4746,7 +4749,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4754,7 +4757,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4777,29 +4780,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <f>B2 / 10</f>
@@ -4808,7 +4811,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -4816,19 +4819,19 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <f xml:space="preserve">  ROUNDUP(B2 / 100, B4)</f>
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1000</v>
@@ -4836,7 +4839,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <f xml:space="preserve"> B7 / 1000</f>
@@ -4845,26 +4848,26 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <f>B7 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <f>B7 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -4875,7 +4878,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <f>B7 * 42</f>
@@ -4903,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -4911,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -4919,7 +4922,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -4927,7 +4930,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -4935,7 +4938,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -4943,7 +4946,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -4951,7 +4954,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -4959,7 +4962,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -4967,7 +4970,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -4975,7 +4978,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -4988,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9897689-B004-4F94-886D-BEFD12E23EE5}">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5000,29 +5003,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <f>B2 / 10</f>
@@ -5031,7 +5034,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <f xml:space="preserve">  ROUNDUP(B2 / 100, 0)</f>
@@ -5040,7 +5043,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -5048,7 +5051,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <f xml:space="preserve"> B6 / 1000</f>
@@ -5057,26 +5060,26 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <f>B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -5087,7 +5090,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>2020</v>
@@ -5095,7 +5098,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <f>B11 / 10</f>
@@ -5114,7 +5117,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -5124,7 +5127,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5132,7 +5135,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5140,7 +5143,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5148,7 +5151,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5156,7 +5159,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5164,7 +5167,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5172,7 +5175,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5180,7 +5183,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5188,7 +5191,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5196,7 +5199,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -5221,7 +5224,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -5236,7 +5239,7 @@
         <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5251,7 +5254,7 @@
         <v>200</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5266,7 +5269,7 @@
         <v>200</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5281,7 +5284,7 @@
         <v>200</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5296,7 +5299,7 @@
         <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5311,7 +5314,7 @@
         <v>200</v>
       </c>
       <c r="D7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5326,7 +5329,7 @@
         <v>200</v>
       </c>
       <c r="D8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5341,7 +5344,7 @@
         <v>200</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5350,7 +5353,7 @@
         <v>100</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -5364,7 +5367,7 @@
     </row>
     <row r="15" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
       <c r="D15" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5391,7 +5394,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -5399,10 +5402,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5410,7 +5413,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5418,7 +5421,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5426,7 +5429,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5434,7 +5437,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5442,7 +5445,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -5450,7 +5453,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -5458,7 +5461,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -5466,7 +5469,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -5495,29 +5498,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1">
         <v>2020</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1">
         <f>B2 / 10</f>
@@ -5526,7 +5529,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <f>ROUNDUP(B2 / 100, 0)</f>
@@ -5535,7 +5538,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>1000</v>
@@ -5543,7 +5546,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <f>B6 / 1000</f>
@@ -5552,26 +5555,26 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1">
         <f>B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -5582,7 +5585,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="1">
         <f>SUM(B2:B4)</f>
@@ -5591,7 +5594,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1">
         <f>SUM(B2:B4) + 2</f>
@@ -5600,7 +5603,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1">
         <f>SUM(B2:B4)</f>
@@ -5622,7 +5625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05739818-17B0-D842-BB6C-69A1E595FDFD}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -5633,7 +5636,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5641,7 +5644,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5649,7 +5652,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5657,7 +5660,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5665,7 +5668,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5673,7 +5676,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5681,7 +5684,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5689,7 +5692,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5697,7 +5700,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5705,7 +5708,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -5713,7 +5716,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -5738,7 +5741,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -5909,7 +5912,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -5917,7 +5920,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5925,7 +5928,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -5933,7 +5936,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5941,7 +5944,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5949,7 +5952,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5957,7 +5960,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5965,7 +5968,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5973,7 +5976,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5981,7 +5984,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -6007,29 +6010,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>2020</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <f>B2 / 10</f>
@@ -6038,7 +6041,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <f xml:space="preserve">  ROUNDUP(B2 / 100, 0)</f>
@@ -6047,7 +6050,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1000</v>
@@ -6055,7 +6058,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <f xml:space="preserve"> B6 / 1000</f>
@@ -6064,26 +6067,26 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <f>B6 * 3.28084</f>
         <v>3280.84</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>B6 * 39.3701</f>
         <v>39370.1</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -6094,7 +6097,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11">
         <v>2020</v>
@@ -6102,7 +6105,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <f>B11 / 10</f>

</xml_diff>